<commit_message>
fix duplicate key run concurency
</commit_message>
<xml_diff>
--- a/CloudTest/SampleData/ChangeAfterAutoCheckOrderTest.xlsx
+++ b/CloudTest/SampleData/ChangeAfterAutoCheckOrderTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LNV\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BE_new\emr-cloud-be\CloudTest\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE62604-8726-4231-B520-53E9E6CD8C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF4F422-2870-44B9-875D-470EF356106A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{1CEC3E68-E8D2-42A2-8922-C523AC6F1661}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1CEC3E68-E8D2-42A2-8922-C523AC6F1661}"/>
   </bookViews>
   <sheets>
     <sheet name="TenMst" sheetId="1" r:id="rId1"/>
@@ -595,9 +595,6 @@
     <t>IS_DELETED</t>
   </si>
   <si>
-    <t>ItemCdTest</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -674,6 +671,9 @@
   </si>
   <si>
     <t>ipnTest</t>
+  </si>
+  <si>
+    <t>ItemCd</t>
   </si>
 </sst>
 </file>
@@ -1028,30 +1028,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4198B0AB-A71B-4C45-B5B9-1132586A5BB4}">
   <dimension ref="A1:GG3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1"/>
-    <col min="15" max="16" width="9.109375" customWidth="1"/>
-    <col min="19" max="19" width="9.109375" customWidth="1"/>
-    <col min="20" max="20" width="13.44140625" customWidth="1"/>
-    <col min="23" max="23" width="9.109375" customWidth="1"/>
-    <col min="146" max="146" width="14.33203125" customWidth="1"/>
-    <col min="154" max="154" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="15" max="16" width="9.140625" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" customWidth="1"/>
+    <col min="23" max="23" width="9.140625" customWidth="1"/>
+    <col min="146" max="146" width="14.28515625" customWidth="1"/>
+    <col min="154" max="154" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:189" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:189" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1620,12 +1620,12 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:189" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:189" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>215</v>
       </c>
       <c r="C2">
         <v>20220403</v>
@@ -1634,22 +1634,22 @@
         <v>20250331</v>
       </c>
       <c r="E2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F2">
         <v>20</v>
       </c>
       <c r="G2" t="s">
+        <v>190</v>
+      </c>
+      <c r="H2" t="s">
         <v>191</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>192</v>
       </c>
-      <c r="I2" t="s">
+      <c r="P2" t="s">
         <v>193</v>
-      </c>
-      <c r="P2" t="s">
-        <v>194</v>
       </c>
       <c r="Q2">
         <v>1</v>
@@ -1661,19 +1661,19 @@
         <v>33</v>
       </c>
       <c r="T2" t="s">
+        <v>194</v>
+      </c>
+      <c r="U2" t="s">
+        <v>194</v>
+      </c>
+      <c r="W2" t="s">
         <v>195</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
         <v>195</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>196</v>
-      </c>
-      <c r="X2" t="s">
-        <v>196</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>197</v>
       </c>
       <c r="Z2">
         <v>1</v>
@@ -1715,7 +1715,7 @@
         <v>0</v>
       </c>
       <c r="AM2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AN2">
         <v>0</v>
@@ -1931,10 +1931,10 @@
         <v>4923</v>
       </c>
       <c r="DX2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="DY2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="DZ2">
         <v>1</v>
@@ -1985,7 +1985,7 @@
         <v>0</v>
       </c>
       <c r="EP2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="EQ2">
         <v>0</v>
@@ -2051,13 +2051,13 @@
         <v>0</v>
       </c>
       <c r="FO2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="FP2">
         <v>99909</v>
       </c>
       <c r="FR2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="FS2">
         <v>99909</v>
@@ -2084,7 +2084,7 @@
         <v>0</v>
       </c>
       <c r="GB2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="GC2">
         <v>0</v>
@@ -2102,12 +2102,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:189" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:189" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C3">
         <v>20220403</v>
@@ -2116,22 +2116,22 @@
         <v>20250331</v>
       </c>
       <c r="E3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F3">
         <v>20</v>
       </c>
       <c r="G3" t="s">
+        <v>190</v>
+      </c>
+      <c r="H3" t="s">
         <v>191</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>192</v>
       </c>
-      <c r="I3" t="s">
+      <c r="P3" t="s">
         <v>193</v>
-      </c>
-      <c r="P3" t="s">
-        <v>194</v>
       </c>
       <c r="Q3">
         <v>1</v>
@@ -2143,19 +2143,19 @@
         <v>33</v>
       </c>
       <c r="T3" t="s">
+        <v>194</v>
+      </c>
+      <c r="U3" t="s">
+        <v>194</v>
+      </c>
+      <c r="W3" t="s">
         <v>195</v>
       </c>
-      <c r="U3" t="s">
+      <c r="X3" t="s">
         <v>195</v>
       </c>
-      <c r="W3" t="s">
+      <c r="Y3" t="s">
         <v>196</v>
-      </c>
-      <c r="X3" t="s">
-        <v>196</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>197</v>
       </c>
       <c r="Z3">
         <v>1</v>
@@ -2197,7 +2197,7 @@
         <v>0</v>
       </c>
       <c r="AM3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AN3">
         <v>0</v>
@@ -2413,7 +2413,7 @@
         <v>4923</v>
       </c>
       <c r="DY3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="DZ3">
         <v>1</v>
@@ -2464,7 +2464,7 @@
         <v>0</v>
       </c>
       <c r="EP3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="EQ3">
         <v>0</v>
@@ -2530,13 +2530,13 @@
         <v>0</v>
       </c>
       <c r="FO3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="FP3">
         <v>99909</v>
       </c>
       <c r="FR3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="FS3">
         <v>99909</v>
@@ -2563,7 +2563,7 @@
         <v>0</v>
       </c>
       <c r="GB3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="GC3">
         <v>0</v>
@@ -2590,66 +2590,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6834CCE-3887-4994-BEAB-3198A45AAA76}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
         <v>202</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>203</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>204</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>205</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>206</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>207</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>208</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>209</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>210</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>211</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>212</v>
       </c>
-      <c r="L1" t="s">
-        <v>213</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2661,7 +2661,7 @@
         <v>99999999</v>
       </c>
       <c r="E2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>